<commit_message>
added further analysis and result tables
</commit_message>
<xml_diff>
--- a/experiments/2022_scientific_reports/results/statistics/stats_effect_cft_interaction.xlsx
+++ b/experiments/2022_scientific_reports/results/statistics/stats_effect_cft_interaction.xlsx
@@ -11,7 +11,7 @@
     <sheet name="normality" sheetId="2" r:id="rId2"/>
     <sheet name="equal_var" sheetId="3" r:id="rId3"/>
     <sheet name="mixed_anova" sheetId="4" r:id="rId4"/>
-    <sheet name="pairwise_ttests" sheetId="5" r:id="rId5"/>
+    <sheet name="pairwise_tests" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -452,7 +452,7 @@
     <t>3.367</t>
   </si>
   <si>
-    <t>Pairwise t-Tests</t>
+    <t>Pairwise Tests</t>
   </si>
 </sst>
 </file>

</xml_diff>